<commit_message>
fix: jar 배포 시 getFile() 접근 불가
- getInputStream()으로 스트림 바로 열어서 사용
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/template.xlsx
+++ b/src/main/resources/templates/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev_yoon\practice_spring_jxls\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD49770E-92B9-4C77-9230-887671137527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96E7499A-481A-49FE-815A-ED55973655C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35670" yWindow="5730" windowWidth="17310" windowHeight="8895" xr2:uid="{83F558C4-28CD-43B3-AD9B-26DA276F8676}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{83F558C4-28CD-43B3-AD9B-26DA276F8676}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -108,15 +108,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>${e.name}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>${e.birthDate}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>${e.payment}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>${e.name}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -541,7 +541,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -564,13 +564,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>